<commit_message>
changed the test data values
</commit_message>
<xml_diff>
--- a/src/main/java/com/automationpractice/testdata/TestDatas.xlsx
+++ b/src/main/java/com/automationpractice/testdata/TestDatas.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14085" windowHeight="6090"/>
   </bookViews>
   <sheets>
     <sheet name="UserRegistration" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -94,21 +95,12 @@
     <t>password1</t>
   </si>
   <si>
-    <t>22-06-1987</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>Sanjay</t>
   </si>
   <si>
-    <t>RoyalCyber</t>
-  </si>
-  <si>
-    <t>Indique</t>
-  </si>
-  <si>
     <t>SRS Plaza</t>
   </si>
   <si>
@@ -118,9 +110,6 @@
     <t>This is an Automation Practice test.</t>
   </si>
   <si>
-    <t>Kathirkamam,Pondicherry</t>
-  </si>
-  <si>
     <t>sanjayganesh@gmail.com</t>
   </si>
   <si>
@@ -133,10 +122,22 @@
     <t>Banaswadi</t>
   </si>
   <si>
-    <t>Kathirkamam,Pondicherry-605009</t>
-  </si>
-  <si>
-    <t>01-05-2016</t>
+    <t>MNC company</t>
+  </si>
+  <si>
+    <t>Outer Ring Road</t>
+  </si>
+  <si>
+    <t>Indian,India</t>
+  </si>
+  <si>
+    <t>Indian ,India,Bangalore</t>
+  </si>
+  <si>
+    <t>12-03-2o11</t>
+  </si>
+  <si>
+    <t>01-05-2014</t>
   </si>
 </sst>
 </file>
@@ -499,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,6 +513,8 @@
     <col min="8" max="8" width="17.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
     <col min="16" max="16" width="14.85546875" customWidth="1"/>
     <col min="18" max="18" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
@@ -601,31 +604,31 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
         <v>27</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
       </c>
       <c r="J2" t="s">
         <v>22</v>
       </c>
       <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
         <v>29</v>
-      </c>
-      <c r="L2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" t="s">
-        <v>32</v>
       </c>
       <c r="O2">
         <v>32</v>
@@ -637,7 +640,7 @@
         <v>21</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S2">
         <v>123456789</v>
@@ -646,7 +649,7 @@
         <v>9987654321</v>
       </c>
       <c r="U2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -654,13 +657,13 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
@@ -669,10 +672,10 @@
         <v>40</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
         <v>22</v>
@@ -681,16 +684,16 @@
         <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="O3">
         <v>32</v>
@@ -702,7 +705,7 @@
         <v>21</v>
       </c>
       <c r="R3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="S3">
         <v>123456789</v>
@@ -711,7 +714,7 @@
         <v>9999999999</v>
       </c>
       <c r="U3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed test data values
</commit_message>
<xml_diff>
--- a/src/main/java/com/automationpractice/testdata/TestDatas.xlsx
+++ b/src/main/java/com/automationpractice/testdata/TestDatas.xlsx
@@ -134,10 +134,10 @@
     <t>Indian ,India,Bangalore</t>
   </si>
   <si>
-    <t>12-03-2o11</t>
-  </si>
-  <si>
     <t>01-05-2014</t>
+  </si>
+  <si>
+    <t>12-03-2011</t>
   </si>
 </sst>
 </file>
@@ -188,11 +188,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,7 +502,7 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,8 +604,8 @@
       <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
-        <v>39</v>
+      <c r="F2" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>
@@ -669,7 +670,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>

</xml_diff>